<commit_message>
Implemented getExpiredCuTru() api, Edited specs
</commit_message>
<xml_diff>
--- a/Specifications (仕様書)/DD (詳細設計)/BackendLogic.xlsx
+++ b/Specifications (仕様書)/DD (詳細設計)/BackendLogic.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>Tên API</t>
   </si>
@@ -201,6 +201,24 @@
         <family val="1"/>
       </rPr>
       <t>hoTen</t>
+    </r>
+  </si>
+  <si>
+    <t>getExpiredCuTrus(hetHan)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lấy ra object CuTru dựa trên param </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>hetHan</t>
     </r>
   </si>
 </sst>
@@ -403,38 +421,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,45 +750,45 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -794,45 +812,45 @@
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -848,14 +866,77 @@
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="19" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A23" s="16"/>
+      <c r="B23" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A24" s="16"/>
+      <c r="B24" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A20:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>